<commit_message>
Update bot for relevant version
</commit_message>
<xml_diff>
--- a/data/Announcements.xlsx
+++ b/data/Announcements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dormitory_bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3178C816-A3AB-4DBA-AB9B-F1AF59602751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE90B2E-7F3D-49D5-9A6D-2A32AAFC0A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,20 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Травля тараканов</t>
-  </si>
-  <si>
-    <t>Смена пропуска</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Название задания</t>
   </si>
   <si>
-    <t>Завоз мебели</t>
-  </si>
-  <si>
     <t>Дата начала</t>
   </si>
   <si>
@@ -51,16 +42,7 @@
     <t>Дополнительная информация</t>
   </si>
   <si>
-    <t>Субботник</t>
-  </si>
-  <si>
     <t>Дата окончания</t>
-  </si>
-  <si>
-    <t>Новые стулья</t>
-  </si>
-  <si>
-    <t>Просим Вас убраться в блоках!</t>
   </si>
 </sst>
 </file>
@@ -414,7 +396,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,98 +411,54 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7">
-        <v>45401</v>
-      </c>
-      <c r="C2" s="7">
-        <v>45401</v>
-      </c>
-      <c r="D2" s="7">
-        <v>45401</v>
-      </c>
-      <c r="E2" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7">
-        <v>45401</v>
-      </c>
-      <c r="C3" s="7">
-        <v>45401</v>
-      </c>
-      <c r="D3" s="7">
-        <v>45401</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.75</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="3"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7">
-        <v>45401</v>
-      </c>
-      <c r="C4" s="7">
-        <v>45401</v>
-      </c>
-      <c r="D4" s="7">
-        <v>45401</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.75347222222222221</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="7">
-        <v>45401</v>
-      </c>
-      <c r="C5" s="7">
-        <v>45401</v>
-      </c>
-      <c r="D5" s="7">
-        <v>45401</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.75694444444444442</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="3"/>
       <c r="F5" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add excel file checker for relevant data about dormitory events by command
</commit_message>
<xml_diff>
--- a/data/Announcements.xlsx
+++ b/data/Announcements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\dormitory_bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE90B2E-7F3D-49D5-9A6D-2A32AAFC0A77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E94347-0C5E-4B03-8674-5E9F6A338C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>